<commit_message>
create terms of reference and project documentation
</commit_message>
<xml_diff>
--- a/documents/Функции и приоритеты.xlsx
+++ b/documents/Функции и приоритеты.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yulia\Study\experience_market\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26114041-1465-4514-BFBE-9B46B9A77A08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC99637F-B597-4739-B547-959020B27494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{AF14DF9E-D3F0-491A-AA0E-2CCA348C55D9}"/>
   </bookViews>
@@ -36,21 +36,12 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
-    <t>Модуль</t>
-  </si>
-  <si>
     <t>Проекты</t>
   </si>
   <si>
     <t>Хакатоны</t>
   </si>
   <si>
-    <t>ЛК</t>
-  </si>
-  <si>
-    <t>Админ панель</t>
-  </si>
-  <si>
     <t>Функции</t>
   </si>
   <si>
@@ -108,15 +99,9 @@
     <t>Создание хакатона вручную</t>
   </si>
   <si>
-    <t>Конкурсы(Челленджи)</t>
-  </si>
-  <si>
     <t>Закрытие конкурса</t>
   </si>
   <si>
-    <t>Ачивки</t>
-  </si>
-  <si>
     <t>Просмотр статистики площадки</t>
   </si>
   <si>
@@ -139,6 +124,21 @@
   </si>
   <si>
     <t xml:space="preserve">Просмотр результатов конкурса </t>
+  </si>
+  <si>
+    <t>Подсистема</t>
+  </si>
+  <si>
+    <t>Система достижений</t>
+  </si>
+  <si>
+    <t>Личный кабинет</t>
+  </si>
+  <si>
+    <t>Конкурсы</t>
+  </si>
+  <si>
+    <t>Административная панель</t>
   </si>
 </sst>
 </file>
@@ -279,7 +279,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -294,48 +294,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -652,42 +649,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4FF57EA-917A-4BB0-A8D5-EC87A9A20155}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22.6328125" customWidth="1"/>
     <col min="2" max="2" width="52.6328125" customWidth="1"/>
-    <col min="3" max="3" width="13" style="17" customWidth="1"/>
+    <col min="3" max="3" width="13" style="10" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="20" t="s">
-        <v>28</v>
+        <v>2</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>23</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
-        <v>1</v>
+      <c r="A2" s="16" t="s">
+        <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C2" s="5">
         <v>1</v>
@@ -699,349 +696,317 @@
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="7"/>
+      <c r="A3" s="17"/>
       <c r="B3" s="5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C3" s="5">
         <v>2</v>
       </c>
-      <c r="D3" s="19"/>
+      <c r="D3" s="14"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="7"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C4" s="5">
         <v>3</v>
       </c>
-      <c r="D4" s="19"/>
+      <c r="D4" s="14"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="7"/>
+      <c r="A5" s="17"/>
       <c r="B5" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C5" s="5">
         <v>4</v>
       </c>
-      <c r="D5" s="19"/>
+      <c r="D5" s="14"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="7"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C6" s="5">
         <v>5</v>
       </c>
-      <c r="D6" s="19"/>
+      <c r="D6" s="14"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="7"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C7" s="5">
         <v>6</v>
       </c>
-      <c r="D7" s="19"/>
+      <c r="D7" s="14"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="8"/>
+      <c r="A8" s="18"/>
       <c r="B8" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C8" s="5">
         <v>7</v>
       </c>
-      <c r="D8" s="14"/>
+      <c r="D8" s="15"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="9"/>
+      <c r="A9" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="11">
+        <v>1</v>
+      </c>
+      <c r="D9" s="13">
+        <v>4</v>
+      </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="17"/>
+      <c r="B10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="11">
         <v>2</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="18">
-        <v>1</v>
-      </c>
-      <c r="D10" s="13">
-        <v>4</v>
-      </c>
+      <c r="D10" s="14"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="7"/>
-      <c r="B11" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="18">
-        <v>2</v>
-      </c>
-      <c r="D11" s="19"/>
+      <c r="A11" s="18"/>
+      <c r="B11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="11">
+        <v>3</v>
+      </c>
+      <c r="D11" s="15"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="8"/>
+      <c r="A12" s="16" t="s">
+        <v>33</v>
+      </c>
       <c r="B12" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="18">
-        <v>3</v>
-      </c>
-      <c r="D12" s="14"/>
+        <v>27</v>
+      </c>
+      <c r="C12" s="11">
+        <v>1</v>
+      </c>
+      <c r="D12" s="13">
+        <v>5</v>
+      </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="9"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="11">
+        <v>2</v>
+      </c>
+      <c r="D13" s="14"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="A14" s="18"/>
       <c r="B14" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="18">
-        <v>1</v>
-      </c>
-      <c r="D14" s="13">
-        <v>5</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="C14" s="11">
+        <v>3</v>
+      </c>
+      <c r="D14" s="15"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="7"/>
+      <c r="A15" s="16" t="s">
+        <v>32</v>
+      </c>
       <c r="B15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="18">
+        <v>12</v>
+      </c>
+      <c r="C15" s="8">
+        <v>1</v>
+      </c>
+      <c r="D15" s="13">
         <v>2</v>
       </c>
-      <c r="D15" s="19"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="8"/>
+      <c r="A16" s="17"/>
       <c r="B16" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="18">
-        <v>3</v>
+        <v>13</v>
+      </c>
+      <c r="C16" s="8">
+        <v>2</v>
       </c>
       <c r="D16" s="14"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="2"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="9"/>
+      <c r="A17" s="17"/>
+      <c r="B17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="11">
+        <v>3</v>
+      </c>
+      <c r="D17" s="14"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="6" t="s">
-        <v>3</v>
-      </c>
+      <c r="A18" s="17"/>
       <c r="B18" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="15">
-        <v>1</v>
-      </c>
-      <c r="D18" s="13">
-        <v>2</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="C18" s="11">
+        <v>4</v>
+      </c>
+      <c r="D18" s="14"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="7"/>
+      <c r="A19" s="18"/>
       <c r="B19" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="15">
-        <v>2</v>
-      </c>
-      <c r="D19" s="19"/>
+        <v>28</v>
+      </c>
+      <c r="C19" s="11">
+        <v>5</v>
+      </c>
+      <c r="D19" s="15"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="7"/>
+      <c r="A20" s="19" t="s">
+        <v>34</v>
+      </c>
       <c r="B20" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="8">
+        <v>1</v>
+      </c>
+      <c r="D20" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="19"/>
+      <c r="B21" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="18">
+      <c r="C21" s="8">
+        <v>2</v>
+      </c>
+      <c r="D21" s="14"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="19"/>
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="8">
         <v>3</v>
       </c>
-      <c r="D20" s="19"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="7"/>
-      <c r="B21" s="3" t="s">
+      <c r="D22" s="14"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="19"/>
+      <c r="B23" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="8">
+        <v>4</v>
+      </c>
+      <c r="D23" s="14"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="19"/>
+      <c r="B24" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="18">
-        <v>4</v>
-      </c>
-      <c r="D21" s="19"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" s="8"/>
-      <c r="B22" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" s="18">
+      <c r="C24" s="8">
         <v>5</v>
       </c>
-      <c r="D22" s="14"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="2"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24" s="15">
-        <v>1</v>
-      </c>
-      <c r="D24" s="13">
-        <v>3</v>
-      </c>
+      <c r="D24" s="14"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="10"/>
-      <c r="B25" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C25" s="15">
-        <v>2</v>
-      </c>
-      <c r="D25" s="19"/>
+      <c r="A25" s="19"/>
+      <c r="B25" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="8">
+        <v>6</v>
+      </c>
+      <c r="D25" s="14"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="10"/>
-      <c r="B26" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" s="15">
-        <v>3</v>
-      </c>
-      <c r="D26" s="19"/>
+      <c r="A26" s="19"/>
+      <c r="B26" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="8">
+        <v>7</v>
+      </c>
+      <c r="D26" s="14"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" s="10"/>
-      <c r="B27" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" s="15">
-        <v>4</v>
-      </c>
-      <c r="D27" s="19"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" s="10"/>
-      <c r="B28" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C28" s="15">
-        <v>5</v>
-      </c>
-      <c r="D28" s="19"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="10"/>
-      <c r="B29" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C29" s="15">
-        <v>6</v>
-      </c>
-      <c r="D29" s="19"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" s="10"/>
-      <c r="B30" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" s="15">
-        <v>7</v>
-      </c>
-      <c r="D30" s="19"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="10"/>
-      <c r="B31" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C31" s="15">
+      <c r="A27" s="19"/>
+      <c r="B27" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="8">
         <v>8</v>
       </c>
-      <c r="D31" s="14"/>
+      <c r="D27" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D24:D31"/>
-    <mergeCell ref="D18:D22"/>
-    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A20:A27"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="D20:D27"/>
+    <mergeCell ref="D15:D19"/>
+    <mergeCell ref="D12:D14"/>
     <mergeCell ref="D2:D8"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A24:A31"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A18:A22"/>
-    <mergeCell ref="A2:A8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>